<commit_message>
Planilla de evaluacion completada por la profe
</commit_message>
<xml_diff>
--- a/Fase 1/Evidencias Grupales/PLANILLA DE EVALUACIÓN FASE 1.xlsx
+++ b/Fase 1/Evidencias Grupales/PLANILLA DE EVALUACIÓN FASE 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/08cad40061c47df9/Documentos/GitHub/Captson_008D-Proyecto-College-Choice-Helper/Fase 1/Evidencias Grupales/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{46B5CC07-EA57-4E50-8FF1-C2568C72DD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC6AE1C8-49F5-453E-99F7-06CF39A068D8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FEFF54-E99F-476F-8C1A-123EDD8E40C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EVALUACION1" sheetId="1" r:id="rId1"/>
@@ -50,21 +50,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="98">
   <si>
     <t>INTEGRANTES</t>
   </si>
@@ -378,16 +369,13 @@
     <t>Muy Relevante</t>
   </si>
   <si>
-    <t>Alexander Hernández</t>
-  </si>
-  <si>
-    <t>Álvaro Muñoz</t>
-  </si>
-  <si>
     <t>Abel Sánchez</t>
   </si>
   <si>
-    <t>X</t>
+    <t xml:space="preserve">Álvaro Muñoz </t>
+  </si>
+  <si>
+    <t>Alexander Hernández</t>
   </si>
 </sst>
 </file>
@@ -1054,6 +1042,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1062,18 +1053,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1153,9 +1141,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1193,7 +1181,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1299,7 +1287,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1441,7 +1429,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1451,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K929"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1501,7 +1489,7 @@
       </c>
       <c r="C4" s="6">
         <f>EVALUACION1!$C$24</f>
-        <v>7</v>
+        <v>6.9</v>
       </c>
       <c r="D4" s="6">
         <f>$C$35</f>
@@ -1509,7 +1497,7 @@
       </c>
       <c r="E4" s="43">
         <f>C4*C$2+D4*D$2</f>
-        <v>7</v>
+        <v>6.9250000000000007</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1522,15 +1510,15 @@
       </c>
       <c r="C5" s="6">
         <f>EVALUACION1!$C$24</f>
-        <v>7</v>
+        <v>6.9</v>
       </c>
       <c r="D5" s="6">
         <f>C47</f>
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="E5" s="43">
         <f t="shared" ref="E5:E6" si="0">C5*C$2+D5*D$2</f>
-        <v>7</v>
+        <v>6.8750000000000009</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1543,15 +1531,15 @@
       </c>
       <c r="C6" s="6">
         <f>EVALUACION1!$C$24</f>
-        <v>7</v>
+        <v>6.9</v>
       </c>
       <c r="D6" s="6">
         <f>C58</f>
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="E6" s="43">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6.8750000000000009</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -1560,22 +1548,22 @@
         <v>3</v>
       </c>
       <c r="B11" s="14"/>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="51" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="60"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="59"/>
     </row>
     <row r="12" spans="1:11" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="62"/>
+      <c r="A12" s="61"/>
       <c r="B12" s="24" t="s">
         <v>6</v>
       </c>
@@ -1583,19 +1571,19 @@
       <c r="D12" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="60"/>
+      <c r="E12" s="59"/>
       <c r="F12" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="60"/>
+      <c r="G12" s="59"/>
       <c r="H12" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="60"/>
+      <c r="I12" s="59"/>
       <c r="J12" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="60"/>
+      <c r="K12" s="59"/>
     </row>
     <row r="13" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="65"/>
@@ -1606,20 +1594,24 @@
       <c r="C13" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>98</v>
+      <c r="D13" s="16" t="str">
+        <f t="shared" ref="D13:D16" si="1">IF($C13=CL,"X","")</f>
+        <v>X</v>
       </c>
       <c r="E13" s="16">
         <f>IF(D13="X",100*0.1,"")</f>
         <v>10</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="16" t="str">
+        <f t="shared" ref="F13:F16" si="2">IF($C13=L,"X","")</f>
+        <v/>
+      </c>
       <c r="G13" s="16" t="str">
         <f>IF(F13="X",60*0.1,"")</f>
         <v/>
       </c>
       <c r="H13" s="16" t="str">
-        <f t="shared" ref="H13:H16" si="1">IF($C13=ML,"X","")</f>
+        <f t="shared" ref="H13:H16" si="3">IF($C13=ML,"X","")</f>
         <v/>
       </c>
       <c r="I13" s="16" t="str">
@@ -1627,11 +1619,11 @@
         <v/>
       </c>
       <c r="J13" s="16" t="str">
-        <f t="shared" ref="J13:J16" si="2">IF($C13=NL,"X","")</f>
+        <f t="shared" ref="J13:J16" si="4">IF($C13=NL,"X","")</f>
         <v/>
       </c>
       <c r="K13" s="16" t="str">
-        <f t="shared" ref="K13:K16" si="3">IF($J13="X",0,"")</f>
+        <f t="shared" ref="K13:K16" si="5">IF($J13="X",0,"")</f>
         <v/>
       </c>
     </row>
@@ -1645,15 +1637,15 @@
         <v>7</v>
       </c>
       <c r="D14" s="16" t="str">
-        <f t="shared" ref="D14:D15" si="4">IF($C14=CL,"X","")</f>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="E14" s="16">
-        <f t="shared" ref="E14" si="5">IF(D14="X",100*0.05,"")</f>
+        <f t="shared" ref="E14" si="6">IF(D14="X",100*0.05,"")</f>
         <v>5</v>
       </c>
       <c r="F14" s="16" t="str">
-        <f t="shared" ref="F14:F15" si="6">IF($C14=L,"X","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G14" s="16" t="str">
@@ -1661,7 +1653,7 @@
         <v/>
       </c>
       <c r="H14" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I14" s="16" t="str">
@@ -1669,11 +1661,11 @@
         <v/>
       </c>
       <c r="J14" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K14" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -1687,7 +1679,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
       <c r="E15" s="16">
@@ -1695,7 +1687,7 @@
         <v>5</v>
       </c>
       <c r="F15" s="16" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="G15" s="16" t="str">
@@ -1703,7 +1695,7 @@
         <v/>
       </c>
       <c r="H15" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I15" s="16" t="str">
@@ -1711,11 +1703,11 @@
         <v/>
       </c>
       <c r="J15" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K15" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -1728,20 +1720,24 @@
       <c r="C16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>98</v>
+      <c r="D16" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>X</v>
       </c>
       <c r="E16" s="16">
         <f>IF(D16="X",100*0.05,"")</f>
         <v>5</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="16" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
       <c r="G16" s="16" t="str">
         <f>IF(F16="X",60*0.05,"")</f>
         <v/>
       </c>
       <c r="H16" s="16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="I16" s="16" t="str">
@@ -1749,11 +1745,11 @@
         <v/>
       </c>
       <c r="J16" s="16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K16" s="16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -1897,8 +1893,7 @@
         <v>X</v>
       </c>
       <c r="E20" s="16">
-        <f>IF(D20="X",100*0.05,"")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F20" s="16" t="str">
         <f t="shared" si="14"/>
@@ -1912,9 +1907,8 @@
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="I20" s="16" t="str">
-        <f t="shared" si="11"/>
-        <v/>
+      <c r="I20" s="16">
+        <v>4</v>
       </c>
       <c r="J20" s="16" t="str">
         <f t="shared" si="18"/>
@@ -2011,18 +2005,18 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="62"/>
+      <c r="A23" s="61"/>
       <c r="B23" s="34" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="37">
         <f>E23+G23+I23+K23</f>
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="19">
         <f>SUM(E13:E22)</f>
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19">
@@ -2032,7 +2026,7 @@
       <c r="H23" s="19"/>
       <c r="I23" s="19">
         <f>SUM(I13:I22)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J23" s="19"/>
       <c r="K23" s="19">
@@ -2047,65 +2041,65 @@
       </c>
       <c r="C24" s="20">
         <f>VLOOKUP(C23,ESCALA_IEP!A2:B142,2,FALSE)</f>
-        <v>7</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="61" t="s">
+      <c r="A27" s="60" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="51" t="str">
+      <c r="C27" s="52" t="str">
         <f>$B$4</f>
-        <v>Alexander Hernández</v>
-      </c>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="53"/>
+        <v>Abel Sánchez</v>
+      </c>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="54"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="62"/>
+      <c r="A28" s="61"/>
       <c r="B28" s="50"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="56"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="57"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="62"/>
+      <c r="A29" s="61"/>
       <c r="B29" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="57" t="s">
+      <c r="C29" s="51" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
-      <c r="K29" s="60"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
+      <c r="K29" s="59"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="62"/>
+      <c r="A30" s="61"/>
       <c r="B30" s="15" t="s">
         <v>6</v>
       </c>
@@ -2113,22 +2107,22 @@
       <c r="D30" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="60"/>
+      <c r="E30" s="59"/>
       <c r="F30" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="60"/>
+      <c r="G30" s="59"/>
       <c r="H30" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="60"/>
+      <c r="I30" s="59"/>
       <c r="J30" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="K30" s="60"/>
+      <c r="K30" s="59"/>
     </row>
     <row r="31" spans="1:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="62"/>
+      <c r="A31" s="61"/>
       <c r="B31" s="35" t="str">
         <f>RUBRICA!A7</f>
         <v>3. Relaciona el Proyecto APT con sus intereses profesionales. *</v>
@@ -2170,7 +2164,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
+      <c r="A32" s="61"/>
       <c r="B32" s="35" t="str">
         <f>RUBRICA!A15</f>
         <v>11. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. *</v>
@@ -2183,17 +2177,13 @@
         <v>X</v>
       </c>
       <c r="E32" s="16">
-        <f>IF(D32="X",100*0.1,"")</f>
         <v>10</v>
       </c>
       <c r="F32" s="16" t="str">
         <f t="shared" si="26"/>
         <v/>
       </c>
-      <c r="G32" s="16" t="str">
-        <f>IF(F32="X",60*0.1,"")</f>
-        <v/>
-      </c>
+      <c r="G32" s="16"/>
       <c r="H32" s="16" t="str">
         <f t="shared" si="27"/>
         <v/>
@@ -2212,7 +2202,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
+      <c r="A33" s="61"/>
       <c r="B33" s="35" t="str">
         <f>RUBRICA!A17</f>
         <v>13. Colaboración y trabajo en equipo *</v>
@@ -2254,7 +2244,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="62"/>
+      <c r="A34" s="61"/>
       <c r="B34" s="21" t="s">
         <v>17</v>
       </c>
@@ -2303,59 +2293,59 @@
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="61" t="s">
+      <c r="A39" s="60" t="s">
         <v>13</v>
       </c>
       <c r="B39" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="51" t="str">
+      <c r="C39" s="52" t="str">
         <f>B5</f>
-        <v>Álvaro Muñoz</v>
-      </c>
-      <c r="D39" s="52"/>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="52"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="53"/>
+        <v xml:space="preserve">Álvaro Muñoz </v>
+      </c>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="54"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="62"/>
+      <c r="A40" s="61"/>
       <c r="B40" s="50"/>
-      <c r="C40" s="54"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="55"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="55"/>
-      <c r="K40" s="56"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="56"/>
+      <c r="J40" s="56"/>
+      <c r="K40" s="57"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="62"/>
+      <c r="A41" s="61"/>
       <c r="B41" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="57" t="s">
+      <c r="C41" s="51" t="s">
         <v>4</v>
       </c>
       <c r="D41" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="E41" s="59"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="59"/>
-      <c r="I41" s="59"/>
-      <c r="J41" s="59"/>
-      <c r="K41" s="60"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="62"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="62"/>
+      <c r="I41" s="62"/>
+      <c r="J41" s="62"/>
+      <c r="K41" s="59"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="62"/>
+      <c r="A42" s="61"/>
       <c r="B42" s="15" t="s">
         <v>6</v>
       </c>
@@ -2363,22 +2353,22 @@
       <c r="D42" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="60"/>
+      <c r="E42" s="59"/>
       <c r="F42" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="60"/>
+      <c r="G42" s="59"/>
       <c r="H42" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="I42" s="60"/>
+      <c r="I42" s="59"/>
       <c r="J42" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="K42" s="60"/>
+      <c r="K42" s="59"/>
     </row>
     <row r="43" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="62"/>
+      <c r="A43" s="61"/>
       <c r="B43" s="35" t="str">
         <f>RUBRICA!A7</f>
         <v>3. Relaciona el Proyecto APT con sus intereses profesionales. *</v>
@@ -2420,7 +2410,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A44" s="62"/>
+      <c r="A44" s="61"/>
       <c r="B44" s="35" t="str">
         <f>RUBRICA!A15</f>
         <v>11. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. *</v>
@@ -2433,8 +2423,7 @@
         <v>X</v>
       </c>
       <c r="E44" s="16">
-        <f>IF(D44="X",100*0.1,"")</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44" s="16" t="str">
         <f t="shared" si="32"/>
@@ -2462,7 +2451,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="62"/>
+      <c r="A45" s="61"/>
       <c r="B45" s="35" t="str">
         <f>RUBRICA!A17</f>
         <v>13. Colaboración y trabajo en equipo *</v>
@@ -2504,18 +2493,18 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="62"/>
+      <c r="A46" s="61"/>
       <c r="B46" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C46" s="18">
         <f>E46+G46+I46+K46</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="19">
         <f>SUM(E43:E45)</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F46" s="19"/>
       <c r="G46" s="19">
@@ -2540,7 +2529,7 @@
       </c>
       <c r="C47" s="20">
         <f>VLOOKUP(C46,ESCALA_TRAB_EQUIP!A2:B62,2,FALSE)</f>
-        <v>7</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2552,59 +2541,59 @@
       <c r="C49" s="23"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="61" t="s">
+      <c r="A50" s="60" t="s">
         <v>13</v>
       </c>
       <c r="B50" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="C50" s="51" t="str">
+      <c r="C50" s="52" t="str">
         <f>B6</f>
-        <v>Abel Sánchez</v>
-      </c>
-      <c r="D50" s="52"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="52"/>
-      <c r="I50" s="52"/>
-      <c r="J50" s="52"/>
-      <c r="K50" s="53"/>
+        <v>Alexander Hernández</v>
+      </c>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="54"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="62"/>
+      <c r="A51" s="61"/>
       <c r="B51" s="50"/>
-      <c r="C51" s="54"/>
-      <c r="D51" s="55"/>
-      <c r="E51" s="55"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="55"/>
-      <c r="H51" s="55"/>
-      <c r="I51" s="55"/>
-      <c r="J51" s="55"/>
-      <c r="K51" s="56"/>
+      <c r="C51" s="55"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="56"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="56"/>
+      <c r="J51" s="56"/>
+      <c r="K51" s="57"/>
     </row>
     <row r="52" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="62"/>
+      <c r="A52" s="61"/>
       <c r="B52" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="57" t="s">
+      <c r="C52" s="51" t="s">
         <v>4</v>
       </c>
       <c r="D52" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="59"/>
-      <c r="F52" s="59"/>
-      <c r="G52" s="59"/>
-      <c r="H52" s="59"/>
-      <c r="I52" s="59"/>
-      <c r="J52" s="59"/>
-      <c r="K52" s="60"/>
+      <c r="E52" s="62"/>
+      <c r="F52" s="62"/>
+      <c r="G52" s="62"/>
+      <c r="H52" s="62"/>
+      <c r="I52" s="62"/>
+      <c r="J52" s="62"/>
+      <c r="K52" s="59"/>
     </row>
     <row r="53" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="62"/>
+      <c r="A53" s="61"/>
       <c r="B53" s="15" t="s">
         <v>6</v>
       </c>
@@ -2612,22 +2601,22 @@
       <c r="D53" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="E53" s="60"/>
+      <c r="E53" s="59"/>
       <c r="F53" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="G53" s="60"/>
+      <c r="G53" s="59"/>
       <c r="H53" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="I53" s="60"/>
+      <c r="I53" s="59"/>
       <c r="J53" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="K53" s="60"/>
+      <c r="K53" s="59"/>
     </row>
     <row r="54" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="62"/>
+      <c r="A54" s="61"/>
       <c r="B54" s="35" t="str">
         <f>RUBRICA!A7</f>
         <v>3. Relaciona el Proyecto APT con sus intereses profesionales. *</v>
@@ -2669,7 +2658,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A55" s="62"/>
+      <c r="A55" s="61"/>
       <c r="B55" s="35" t="str">
         <f>RUBRICA!A15</f>
         <v>11. Expone el tema utilizando un lenguaje técnico disciplinar al presentar la propuesta y responde evidenciando un manejo de la información. *</v>
@@ -2682,8 +2671,7 @@
         <v>X</v>
       </c>
       <c r="E55" s="16">
-        <f>IF(D55="X",100*0.1,"")</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" s="16" t="str">
         <f t="shared" si="40"/>
@@ -2711,7 +2699,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="62"/>
+      <c r="A56" s="61"/>
       <c r="B56" s="35" t="str">
         <f>RUBRICA!A17</f>
         <v>13. Colaboración y trabajo en equipo *</v>
@@ -2753,13 +2741,13 @@
       </c>
     </row>
     <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="62"/>
+      <c r="A57" s="61"/>
       <c r="B57" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C57" s="18">
         <f>E57+G57+I57+K57</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D57" s="19">
         <f>COUNTIF(D55:D56,"X")</f>
@@ -2767,7 +2755,7 @@
       </c>
       <c r="E57" s="19">
         <f>SUM(E54:E56)</f>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F57" s="19">
         <f t="shared" ref="F57" si="44">SUM(F54:F56)</f>
@@ -2801,7 +2789,7 @@
       </c>
       <c r="C58" s="20">
         <f>VLOOKUP(C57,ESCALA_TRAB_EQUIP!A2:B62,2,FALSE)</f>
-        <v>7</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3680,17 +3668,14 @@
     <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C50:K51"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="A50:A58"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="D52:K52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:K40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:K41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
     <mergeCell ref="A39:A47"/>
     <mergeCell ref="A27:A35"/>
     <mergeCell ref="E2:E3"/>
@@ -3707,14 +3692,17 @@
     <mergeCell ref="D29:K29"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="F30:G30"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:K40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:K41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="D52:K52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C50:K51"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="A50:A58"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:E6">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">

</xml_diff>